<commit_message>
update RPS_test.py(주석 추가), modify test_result.xlsx(승률 수정)
</commit_message>
<xml_diff>
--- a/test_result.xlsx
+++ b/test_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timbe\Documents\Programming\RockPaperScissors_AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E680B6-D1D0-49FF-8200-F39FACA14045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91207A92-B330-497B-8E03-C77B41035CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDD74F71-5213-4863-9533-D920D5526CBB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
   <si>
     <t>case1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>컴퓨터 승률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>민경진(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>민경진(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>민경진(3)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -446,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C50B55-7A81-4CEE-892F-EB57920A18CD}">
-  <dimension ref="C3:M37"/>
+  <dimension ref="C3:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -773,452 +785,547 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f>AVERAGE(G4:G13)</f>
+        <v>63.335000000000001</v>
+      </c>
+      <c r="H14">
+        <f>AVERAGE(H4:H13)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>11</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>12</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>48</v>
-      </c>
-      <c r="F16">
-        <v>50</v>
-      </c>
-      <c r="G16">
-        <v>100</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ref="H16:H25" si="1">E16/F16*100</f>
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>48</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ref="H17:H26" si="1">E17/F17*100</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
         <v>1</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>17</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>32</v>
       </c>
-      <c r="F17">
-        <v>50</v>
-      </c>
-      <c r="G17">
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18">
         <v>65.31</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>10</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>28</v>
       </c>
-      <c r="F18">
-        <v>50</v>
-      </c>
-      <c r="G18">
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19">
         <v>73.680000000000007</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <f t="shared" si="1"/>
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
         <v>3</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>27</v>
       </c>
-      <c r="F19">
-        <v>50</v>
-      </c>
-      <c r="G19">
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
         <v>93.1</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
         <v>4</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>32</v>
       </c>
-      <c r="F20">
-        <v>50</v>
-      </c>
-      <c r="G20">
-        <v>100</v>
-      </c>
-      <c r="H20">
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>37</v>
       </c>
-      <c r="F21">
-        <v>50</v>
-      </c>
-      <c r="G21">
-        <v>100</v>
-      </c>
-      <c r="H21">
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
         <v>6</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>16</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>34</v>
       </c>
-      <c r="F22">
-        <v>50</v>
-      </c>
-      <c r="G22">
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
         <v>68</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <v>6</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>8</v>
       </c>
-      <c r="F23">
-        <v>50</v>
-      </c>
-      <c r="G23">
+      <c r="F24">
+        <v>50</v>
+      </c>
+      <c r="G24">
         <v>57.14</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
         <v>8</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>13</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>27</v>
       </c>
-      <c r="F24">
-        <v>50</v>
-      </c>
-      <c r="G24">
+      <c r="F25">
+        <v>50</v>
+      </c>
+      <c r="G25">
         <v>67.5</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
         <v>9</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>1</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>25</v>
       </c>
-      <c r="F25">
-        <v>50</v>
-      </c>
-      <c r="G25">
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26">
         <v>96.15</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
+      <c r="G27">
+        <f>AVERAGE(G17:G26)</f>
+        <v>82.087999999999994</v>
+      </c>
+      <c r="H27">
+        <f>AVERAGE(H17:H26)</f>
+        <v>59.6</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
         <v>10</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>11</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F29" t="s">
         <v>12</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>0</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <v>49</v>
       </c>
-      <c r="F28">
-        <v>50</v>
-      </c>
-      <c r="G28">
-        <v>100</v>
-      </c>
-      <c r="H28">
-        <f t="shared" ref="H28:H37" si="2">E28/F28*100</f>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>100</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ref="H30:H39" si="2">E30/F30*100</f>
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
         <v>1</v>
       </c>
-      <c r="D29">
+      <c r="D31">
         <v>16</v>
       </c>
-      <c r="E29">
+      <c r="E31">
         <v>34</v>
       </c>
-      <c r="F29">
-        <v>50</v>
-      </c>
-      <c r="G29">
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31">
         <v>68</v>
       </c>
-      <c r="H29">
+      <c r="H31">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
         <v>2</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <v>12</v>
       </c>
-      <c r="E30">
+      <c r="E32">
         <v>20</v>
       </c>
-      <c r="F30">
-        <v>50</v>
-      </c>
-      <c r="G30">
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="G32">
         <v>62.5</v>
       </c>
-      <c r="H30">
+      <c r="H32">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
         <v>3</v>
       </c>
-      <c r="D31">
+      <c r="D33">
         <v>27</v>
       </c>
-      <c r="E31">
+      <c r="E33">
         <v>3</v>
       </c>
-      <c r="F31">
-        <v>50</v>
-      </c>
-      <c r="G31">
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33">
         <v>10</v>
       </c>
-      <c r="H31">
+      <c r="H33">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
         <v>4</v>
       </c>
-      <c r="D32">
+      <c r="D34">
         <v>9</v>
       </c>
-      <c r="E32">
+      <c r="E34">
         <v>32</v>
       </c>
-      <c r="F32">
-        <v>50</v>
-      </c>
-      <c r="G32">
+      <c r="F34">
+        <v>50</v>
+      </c>
+      <c r="G34">
         <v>78.05</v>
       </c>
-      <c r="H32">
+      <c r="H34">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
         <v>5</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <v>12</v>
       </c>
-      <c r="E33">
+      <c r="E35">
         <v>25</v>
       </c>
-      <c r="F33">
-        <v>50</v>
-      </c>
-      <c r="G33">
+      <c r="F35">
+        <v>50</v>
+      </c>
+      <c r="G35">
         <v>67.569999999999993</v>
       </c>
-      <c r="H33">
+      <c r="H35">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
         <v>6</v>
       </c>
-      <c r="D34">
+      <c r="D36">
         <v>24</v>
       </c>
-      <c r="E34">
+      <c r="E36">
         <v>26</v>
       </c>
-      <c r="F34">
-        <v>50</v>
-      </c>
-      <c r="G34">
+      <c r="F36">
+        <v>50</v>
+      </c>
+      <c r="G36">
         <v>52</v>
       </c>
-      <c r="H34">
+      <c r="H36">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
         <v>7</v>
       </c>
-      <c r="D35">
+      <c r="D37">
         <v>12</v>
       </c>
-      <c r="E35">
+      <c r="E37">
         <v>0</v>
       </c>
-      <c r="F35">
-        <v>50</v>
-      </c>
-      <c r="G35">
+      <c r="F37">
+        <v>50</v>
+      </c>
+      <c r="G37">
         <v>0</v>
       </c>
-      <c r="H35">
+      <c r="H37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
         <v>8</v>
       </c>
-      <c r="D36">
+      <c r="D38">
         <v>0</v>
       </c>
-      <c r="E36">
+      <c r="E38">
         <v>37</v>
       </c>
-      <c r="F36">
-        <v>50</v>
-      </c>
-      <c r="G36">
-        <v>100</v>
-      </c>
-      <c r="H36">
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+      <c r="H38">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
         <v>9</v>
       </c>
-      <c r="D37">
+      <c r="D39">
         <v>8</v>
       </c>
-      <c r="E37">
+      <c r="E39">
         <v>17</v>
       </c>
-      <c r="F37">
-        <v>50</v>
-      </c>
-      <c r="G37">
+      <c r="F39">
+        <v>50</v>
+      </c>
+      <c r="G39">
         <v>68</v>
       </c>
-      <c r="H37">
+      <c r="H39">
         <f t="shared" si="2"/>
         <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f>AVERAGE(G30:G39)</f>
+        <v>60.612000000000002</v>
+      </c>
+      <c r="H40">
+        <f>AVERAGE(H30:H39)</f>
+        <v>48.6</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>29</v>
+      </c>
+      <c r="E48">
+        <v>39</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
+      </c>
+      <c r="G48">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>26</v>
+      </c>
+      <c r="E49">
+        <v>41</v>
+      </c>
+      <c r="F49">
+        <v>100</v>
+      </c>
+      <c r="G49">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50">
+        <v>25</v>
+      </c>
+      <c r="E50">
+        <v>52</v>
+      </c>
+      <c r="F50">
+        <v>100</v>
+      </c>
+      <c r="G50">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>